<commit_message>
Inputs for Activators in the spreadsheet can now be either name or number
</commit_message>
<xml_diff>
--- a/Livestream.xlsx
+++ b/Livestream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livestream\go\pkg\mod\github.com\lobosat\APCvmix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F566F519-072D-46B3-AFEE-A0537CD1A401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CE8F02-24B6-4484-94DC-A393F64D670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="1050" windowWidth="18900" windowHeight="8475" tabRatio="844" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="1215" windowWidth="18900" windowHeight="8475" tabRatio="844" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prayers" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="284">
   <si>
     <t>Button</t>
   </si>
@@ -4506,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4567,8 +4567,8 @@
       <c r="B2" s="66">
         <v>1</v>
       </c>
-      <c r="C2" s="66">
-        <v>22</v>
+      <c r="C2" s="66" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="66">
         <v>5</v>
@@ -4666,8 +4666,8 @@
       <c r="B5" s="66">
         <v>2</v>
       </c>
-      <c r="C5" s="66">
-        <v>23</v>
+      <c r="C5" s="66" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="66">
         <v>6</v>
@@ -4729,8 +4729,8 @@
       <c r="B8" s="66">
         <v>3</v>
       </c>
-      <c r="C8" s="66">
-        <v>28</v>
+      <c r="C8" s="66" t="s">
+        <v>175</v>
       </c>
       <c r="D8" s="66">
         <v>7</v>
@@ -4847,8 +4847,8 @@
         <v>1</v>
       </c>
       <c r="B14" s="66"/>
-      <c r="C14" s="66">
-        <v>30</v>
+      <c r="C14" s="66" t="s">
+        <v>47</v>
       </c>
       <c r="D14" s="66">
         <v>15</v>
@@ -4904,8 +4904,8 @@
         <v>1</v>
       </c>
       <c r="B17" s="66"/>
-      <c r="C17" s="66">
-        <v>31</v>
+      <c r="C17" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="D17" s="66"/>
       <c r="E17" s="66"/>

</xml_diff>

<commit_message>
Determine textbox name for text overlays from the vmix xml
</commit_message>
<xml_diff>
--- a/Livestream.xlsx
+++ b/Livestream.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livestream\go\pkg\mod\github.com\lobosat\APCvmix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CE8F02-24B6-4484-94DC-A393F64D670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC97511-4239-45B4-9AF0-2BB8434257EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="1215" windowWidth="18900" windowHeight="8475" tabRatio="844" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="1215" windowWidth="18900" windowHeight="8475" tabRatio="844" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prayers" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="281">
   <si>
     <t>Button</t>
   </si>
@@ -446,12 +446,6 @@
   </si>
   <si>
     <t>Thanks be to God</t>
-  </si>
-  <si>
-    <t>red: 1</t>
-  </si>
-  <si>
-    <t>off: 1</t>
   </si>
   <si>
     <t>Overlay1</t>
@@ -914,9 +908,6 @@
   <si>
     <t>ScriptStart Value=OpeningStart
 leds yellowBlink 55</t>
-  </si>
-  <si>
-    <t>leds yellow 55</t>
   </si>
   <si>
     <t>greenBlink: 19</t>
@@ -1930,7 +1921,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>40</v>
@@ -1950,10 +1941,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E2" s="51" t="s">
         <v>42</v>
@@ -1987,7 +1978,7 @@
         <v>36</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>10</v>
@@ -1995,7 +1986,7 @@
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="G4" s="52" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="63.75">
@@ -2003,15 +1994,15 @@
         <v>37</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E5" s="51"/>
       <c r="G5" s="51" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="63.75">
@@ -2019,11 +2010,11 @@
         <v>38</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="51"/>
@@ -2034,11 +2025,11 @@
         <v>39</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C7" s="51"/>
       <c r="D7" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
@@ -2046,27 +2037,27 @@
     </row>
     <row r="8" spans="1:7">
       <c r="D8" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="D9" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="D10" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5">
       <c r="D11" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="76.5">
       <c r="D12" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2303,7 +2294,7 @@
         <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2349,7 +2340,7 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2395,7 +2386,7 @@
         <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2679,7 +2670,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>3</v>
@@ -2687,31 +2678,31 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="38">
         <v>54</v>
@@ -2719,7 +2710,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B6" s="38">
         <v>55</v>
@@ -2727,7 +2718,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B7" s="38">
         <v>56</v>
@@ -2787,25 +2778,25 @@
         <v>41</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" thickBot="1">
@@ -2836,126 +2827,126 @@
     </row>
     <row r="4" spans="1:8" ht="51">
       <c r="B4" s="48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G4" s="48" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H4" s="48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="63.75">
       <c r="B5" s="48" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" s="48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F5" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="G5" s="48" t="s">
-        <v>205</v>
-      </c>
       <c r="H5" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="76.5">
       <c r="B6" s="48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G6" s="48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="51">
       <c r="B7" s="48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="76.5">
       <c r="B8" s="48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="76.5">
       <c r="B9" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>160</v>
-      </c>
       <c r="D9" s="48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="76.5">
       <c r="B10" s="48" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="25.5">
       <c r="C11" s="48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2988,7 +2979,7 @@
         <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -3002,13 +2993,13 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
@@ -3019,13 +3010,13 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3036,30 +3027,30 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.5">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3632,10 +3623,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3643,10 +3634,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3654,7 +3645,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3665,7 +3656,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
         <v>133</v>
@@ -3676,10 +3667,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3687,10 +3678,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3698,10 +3689,10 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3709,10 +3700,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3720,10 +3711,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3731,10 +3722,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="38.25">
@@ -3742,10 +3733,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3753,10 +3744,10 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3764,10 +3755,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3784,8 +3775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IW90"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3866,7 +3857,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>67</v>
@@ -3878,7 +3869,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>66</v>
@@ -3891,7 +3882,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>64</v>
@@ -3904,7 +3895,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>79</v>
@@ -3961,7 +3952,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>44</v>
@@ -3980,13 +3971,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -4004,10 +3995,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4015,7 +4006,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>6</v>
@@ -4030,19 +4021,22 @@
       <c r="A27" s="14">
         <v>26</v>
       </c>
+      <c r="B27" s="15" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="14">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4075,10 +4069,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4101,10 +4095,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>40</v>
@@ -4120,10 +4114,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>46</v>
@@ -4139,7 +4133,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>127</v>
@@ -4150,10 +4144,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4181,10 +4175,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -4197,7 +4191,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>48</v>
@@ -4213,13 +4207,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -4238,6 +4232,9 @@
       <c r="A55" s="14">
         <v>54</v>
       </c>
+      <c r="B55" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4">
@@ -4245,7 +4242,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>269</v>
+        <v>73</v>
       </c>
       <c r="D56" s="14"/>
     </row>
@@ -4253,6 +4250,9 @@
       <c r="A57" s="14">
         <v>56</v>
       </c>
+      <c r="B57" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="D57" s="14"/>
     </row>
     <row r="58" spans="1:4">
@@ -4305,10 +4305,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -4316,10 +4316,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -4327,10 +4327,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -4338,10 +4338,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -4349,10 +4349,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -4360,10 +4360,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -4371,10 +4371,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -4382,7 +4382,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -4390,7 +4390,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>115</v>
@@ -4404,7 +4404,7 @@
         <v>17</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -4506,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4551,13 +4551,13 @@
         <v>17</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4589,9 +4589,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="69"/>
-      <c r="K2" s="70">
-        <v>49</v>
-      </c>
+      <c r="K2" s="70"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="71" t="s">
@@ -4601,30 +4599,28 @@
         <v>50</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G3" s="59" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I3" s="53" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="72" t="s">
-        <v>134</v>
-      </c>
+      <c r="K3" s="72"/>
     </row>
     <row r="4" spans="1:11" ht="13.5" thickBot="1">
       <c r="A4" s="73" t="s">
@@ -4634,30 +4630,28 @@
         <v>51</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="74" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G4" s="76" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H4" s="74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I4" s="74" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="74"/>
-      <c r="K4" s="77" t="s">
-        <v>135</v>
-      </c>
+      <c r="K4" s="77"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="65" t="s">
@@ -4688,7 +4682,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>26</v>
@@ -4709,7 +4703,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>27</v>
@@ -4730,7 +4724,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D8" s="66">
         <v>7</v>
@@ -4751,7 +4745,7 @@
         <v>56</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>28</v>
@@ -4772,7 +4766,7 @@
         <v>57</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D10" s="74" t="s">
         <v>29</v>
@@ -4791,7 +4785,7 @@
       </c>
       <c r="B11" s="66"/>
       <c r="C11" s="66" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D11" s="66">
         <v>8</v>
@@ -4810,10 +4804,10 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="64" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9"/>
@@ -4829,10 +4823,10 @@
       </c>
       <c r="B13" s="74"/>
       <c r="C13" s="78" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D13" s="74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E13" s="74"/>
       <c r="F13" s="74"/>
@@ -4867,10 +4861,10 @@
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -4886,10 +4880,10 @@
       </c>
       <c r="B16" s="78"/>
       <c r="C16" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D16" s="74" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E16" s="78"/>
       <c r="F16" s="74"/>
@@ -4922,7 +4916,7 @@
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -4939,7 +4933,7 @@
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="74" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D19" s="78"/>
       <c r="E19" s="78"/>

</xml_diff>

<commit_message>
Before simplifying MIDI initialization processes
</commit_message>
<xml_diff>
--- a/Livestream.xlsx
+++ b/Livestream.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livestream\go\pkg\mod\github.com\lobosat\APCvmix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC97511-4239-45B4-9AF0-2BB8434257EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4CFC6-6890-4241-9701-A60452058736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="1215" windowWidth="18900" windowHeight="8475" tabRatio="844" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5265" yWindow="2115" windowWidth="18900" windowHeight="12315" tabRatio="844" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prayers" sheetId="2" r:id="rId1"/>
-    <sheet name="Hymns" sheetId="7" r:id="rId2"/>
-    <sheet name="Speakers" sheetId="12" r:id="rId3"/>
-    <sheet name="cameras" sheetId="11" r:id="rId4"/>
-    <sheet name="microphones" sheetId="10" r:id="rId5"/>
+    <sheet name="Hymns" sheetId="7" r:id="rId1"/>
+    <sheet name="Speakers" sheetId="12" r:id="rId2"/>
+    <sheet name="Prayers" sheetId="2" r:id="rId3"/>
+    <sheet name="microphones" sheetId="10" r:id="rId4"/>
+    <sheet name="cameras" sheetId="11" r:id="rId5"/>
     <sheet name="Responses" sheetId="1" r:id="rId6"/>
     <sheet name="Shortcuts" sheetId="4" r:id="rId7"/>
     <sheet name="Activators" sheetId="3" r:id="rId8"/>
     <sheet name="Faders" sheetId="5" r:id="rId9"/>
     <sheet name="Initial State" sheetId="8" r:id="rId10"/>
-    <sheet name="Config" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="271">
   <si>
     <t>Button</t>
   </si>
@@ -55,9 +54,6 @@
     <t>Response</t>
   </si>
   <si>
-    <t>Response.Text</t>
-  </si>
-  <si>
     <t>Amen</t>
   </si>
   <si>
@@ -457,30 +453,6 @@
     <t>on: 71</t>
   </si>
   <si>
-    <t>Prayers textbox name</t>
-  </si>
-  <si>
-    <t>Hymns textbox name</t>
-  </si>
-  <si>
-    <t>Lector textbox name</t>
-  </si>
-  <si>
-    <t>Prev button</t>
-  </si>
-  <si>
-    <t>Next button</t>
-  </si>
-  <si>
-    <t>OvOff button</t>
-  </si>
-  <si>
-    <t>Textbox.Text</t>
-  </si>
-  <si>
-    <t>Response textbox name</t>
-  </si>
-  <si>
     <t>PoP</t>
   </si>
   <si>
@@ -494,9 +466,6 @@
   </si>
   <si>
     <t>HebrewStart</t>
-  </si>
-  <si>
-    <t>lyrics.Text</t>
   </si>
   <si>
     <t>Lift every voice and sing till earth and heaven ring
@@ -1310,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1386,9 +1355,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1894,179 +1860,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804F0BF0-44B3-4553-A5BB-CBA05E193E99}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="32" style="4" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" style="4" customWidth="1"/>
-    <col min="8" max="1026" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="44"/>
+    <col min="2" max="2" width="44.140625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="47" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="47" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="47" customWidth="1"/>
+    <col min="8" max="8" width="41" style="47" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="50"/>
-      <c r="B1" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="51" t="s">
+    <row r="1" spans="1:8" ht="13.5" thickBot="1">
+      <c r="B1" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="51" t="s">
+      <c r="B2" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13.5" thickBot="1">
+      <c r="A3" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="42">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="50" t="s">
+      <c r="C3" s="43">
+        <v>18</v>
+      </c>
+      <c r="D3" s="43">
+        <v>33</v>
+      </c>
+      <c r="E3" s="43">
+        <v>37</v>
+      </c>
+      <c r="F3" s="43">
+        <v>39</v>
+      </c>
+      <c r="G3" s="43">
         <v>41</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="H3" s="48">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="51">
+      <c r="B4" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>269</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63.75">
+      <c r="B5" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="76.5">
+      <c r="B6" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51">
+      <c r="B7" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="76.5">
+      <c r="B8" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="76.5">
+      <c r="B9" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="51" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="51">
-        <v>24</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51">
-        <v>25</v>
-      </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="165.75">
-      <c r="A4" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="G4" s="52" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63.75">
-      <c r="A5" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="G5" s="51" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="63.75">
-      <c r="A6" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-    </row>
-    <row r="7" spans="1:7" ht="76.5">
-      <c r="A7" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="D8" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="D10" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="25.5">
-      <c r="D11" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="76.5">
-      <c r="D12" s="4" t="s">
-        <v>190</v>
+      <c r="C9" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="47" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="76.5">
+      <c r="B10" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="25.5">
+      <c r="C11" s="47" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2074,7 +2089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFA0029-6F67-4CFC-9DD5-769ABDA5C3FC}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2088,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2109,10 +2124,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2120,10 +2135,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2131,10 +2146,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2142,10 +2157,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2153,10 +2168,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2164,10 +2179,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2175,10 +2190,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2206,10 +2221,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2217,10 +2232,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2228,10 +2243,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2239,10 +2254,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2250,7 +2265,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2258,7 +2273,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2291,10 +2306,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2337,10 +2352,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2383,10 +2398,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2419,10 +2434,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2435,10 +2450,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2466,10 +2481,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
         <v>71</v>
-      </c>
-      <c r="C55" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2477,10 +2492,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2488,10 +2503,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2504,10 +2519,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2515,10 +2530,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2526,10 +2541,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2547,10 +2562,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2558,10 +2573,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2647,81 +2662,6 @@
     <row r="82" spans="1:1">
       <c r="A82">
         <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4907AA9-3DC8-4BF4-8885-8E651EC1BA62}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="38" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" s="38">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="38">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" s="38">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2730,232 +2670,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804F0BF0-44B3-4553-A5BB-CBA05E193E99}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="45"/>
-    <col min="2" max="2" width="44.140625" style="48" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="48" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="48" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="48" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="48" customWidth="1"/>
-    <col min="8" max="8" width="41" style="48" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="45"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1">
-      <c r="B1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="43">
-        <v>9</v>
-      </c>
-      <c r="C3" s="44">
-        <v>18</v>
-      </c>
-      <c r="D3" s="44">
-        <v>33</v>
-      </c>
-      <c r="E3" s="44">
-        <v>37</v>
-      </c>
-      <c r="F3" s="44">
-        <v>39</v>
-      </c>
-      <c r="G3" s="44">
-        <v>41</v>
-      </c>
-      <c r="H3" s="49">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="51">
-      <c r="B4" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>279</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75">
-      <c r="B5" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="76.5">
-      <c r="B6" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>204</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="51">
-      <c r="B7" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="G7" s="48" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="76.5">
-      <c r="B8" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>206</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="76.5">
-      <c r="B9" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="G9" s="48" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="76.5">
-      <c r="B10" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="25.5">
-      <c r="C11" s="48" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11E46E2-E41B-4167-9FB7-A206252B61D0}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2976,81 +2690,81 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>168</v>
+        <v>140</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.5">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>187</v>
+        <v>162</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3058,263 +2772,210 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4C6AC8-1F71-4368-A31F-D9706EF042E2}">
-  <dimension ref="A1:G15"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D18:D19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="32" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" style="4" customWidth="1"/>
+    <col min="8" max="1026" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
-      <c r="A1" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75">
-      <c r="A2" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75">
-      <c r="A4" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75">
-      <c r="A5" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75">
-      <c r="A6" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75">
-      <c r="A7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="1"/>
-      <c r="C11" s="36"/>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="1"/>
-      <c r="C12" s="36"/>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="1"/>
-      <c r="C13" s="36"/>
-      <c r="F13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="1"/>
-      <c r="C14" s="36"/>
-      <c r="F14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="1"/>
-      <c r="C15" s="36"/>
+    <row r="1" spans="1:7">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="50">
+        <v>24</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50">
+        <v>25</v>
+      </c>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="165.75">
+      <c r="A4" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="G4" s="51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="63.75">
+      <c r="A5" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="50"/>
+      <c r="G5" s="50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63.75">
+      <c r="A6" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+    </row>
+    <row r="7" spans="1:7" ht="76.5">
+      <c r="A7" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="25.5">
+      <c r="D11" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="76.5">
+      <c r="D12" s="4" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10 D2:D10" xr:uid="{28CCA215-10A7-43AC-95BD-7C8CC9D13F72}">
-      <formula1>$F$10:$F$16</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{3BD83D5C-14E7-4332-BAE4-F4B7ED230554}">
-      <formula1>$F$3:$F$8</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EB5AB2-6FA1-46DC-9DC0-AB3C2D9EA56A}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>1</v>
@@ -3322,230 +2983,230 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="25"/>
       <c r="H2" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="25"/>
       <c r="H3" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="25"/>
       <c r="H4" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="25"/>
       <c r="H5" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>88</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>89</v>
       </c>
       <c r="F6" s="25"/>
       <c r="H6" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>91</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>92</v>
       </c>
       <c r="F7" s="25"/>
       <c r="H7" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15">
       <c r="A8" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>94</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>95</v>
       </c>
       <c r="F8" s="25"/>
       <c r="H8" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>97</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>98</v>
       </c>
       <c r="F9" s="25"/>
       <c r="H9" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>100</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>101</v>
       </c>
       <c r="F10" s="25"/>
       <c r="H10" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="A11" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>103</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>104</v>
       </c>
       <c r="F11" s="25"/>
       <c r="H11" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>106</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>107</v>
       </c>
       <c r="F12" s="25"/>
       <c r="H12" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1">
       <c r="A13" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>109</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>110</v>
       </c>
       <c r="F13" s="25"/>
       <c r="H13" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" thickBot="1">
@@ -3555,19 +3216,19 @@
       <c r="E14" s="29"/>
       <c r="F14" s="25"/>
       <c r="H14" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="25"/>
       <c r="H15" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="25"/>
       <c r="H16" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -3592,12 +3253,244 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4C6AC8-1F71-4368-A31F-D9706EF042E2}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75">
+      <c r="A1" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
+      <c r="A2" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75">
+      <c r="A3" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
+      <c r="A4" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="A6" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75">
+      <c r="A7" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75">
+      <c r="A8" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75">
+      <c r="A9" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75">
+      <c r="A10" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="1"/>
+      <c r="C11" s="36"/>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="1"/>
+      <c r="C12" s="36"/>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="1"/>
+      <c r="C13" s="36"/>
+      <c r="F13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="1"/>
+      <c r="C14" s="36"/>
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="1"/>
+      <c r="C15" s="36"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10 D2:D10" xr:uid="{28CCA215-10A7-43AC-95BD-7C8CC9D13F72}">
+      <formula1>$F$10:$F$16</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{3BD83D5C-14E7-4332-BAE4-F4B7ED230554}">
+      <formula1>$F$3:$F$8</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3612,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3623,10 +3516,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3634,10 +3527,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3645,10 +3538,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3656,10 +3549,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3667,10 +3560,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3678,10 +3571,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3689,10 +3582,10 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3700,10 +3593,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3711,10 +3604,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3722,10 +3615,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="38.25">
@@ -3733,10 +3626,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>200</v>
+        <v>167</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3744,10 +3637,10 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3755,10 +3648,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3775,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IW90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -3797,13 +3690,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3821,10 +3714,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -3833,10 +3726,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -3845,10 +3738,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -3857,10 +3750,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -3869,10 +3762,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13"/>
@@ -3882,10 +3775,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -3895,10 +3788,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="11"/>
     </row>
@@ -3944,7 +3837,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5">
@@ -3952,10 +3845,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3963,7 +3856,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3971,13 +3864,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3995,10 +3888,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4006,10 +3899,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4022,7 +3915,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4030,13 +3923,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4069,10 +3962,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4095,13 +3988,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -4114,13 +4007,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -4133,10 +4026,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -4144,10 +4037,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4175,10 +4068,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -4191,10 +4084,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -4207,13 +4100,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>263</v>
-      </c>
       <c r="D52" s="14" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -4233,7 +4126,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D55" s="14"/>
     </row>
@@ -4242,7 +4135,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" s="14"/>
     </row>
@@ -4251,7 +4144,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D57" s="14"/>
     </row>
@@ -4266,7 +4159,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="14"/>
     </row>
@@ -4275,7 +4168,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="14"/>
     </row>
@@ -4284,7 +4177,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="14"/>
     </row>
@@ -4305,10 +4198,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -4316,10 +4209,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -4327,10 +4220,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -4338,10 +4231,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -4349,10 +4242,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -4360,10 +4253,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -4371,10 +4264,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -4382,7 +4275,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -4390,10 +4283,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -4401,10 +4294,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -4527,165 +4420,165 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="65">
+        <v>1</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="65">
+        <v>5</v>
+      </c>
+      <c r="E2" s="65">
+        <v>26</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="68"/>
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="I3" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="65" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="71"/>
+    </row>
+    <row r="4" spans="1:11" ht="13.5" thickBot="1">
+      <c r="A4" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="73"/>
+      <c r="K4" s="76"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66">
-        <v>1</v>
-      </c>
-      <c r="C2" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="66">
-        <v>5</v>
-      </c>
-      <c r="E2" s="66">
-        <v>26</v>
-      </c>
-      <c r="F2" s="67" t="s">
+      <c r="B5" s="65">
+        <v>2</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="65">
+        <v>6</v>
+      </c>
+      <c r="E5" s="65"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
+    </row>
+    <row r="6" spans="1:11" ht="25.5">
+      <c r="A6" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="69"/>
-      <c r="K2" s="70"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A4" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="74" t="s">
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="74" t="s">
-        <v>268</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>259</v>
-      </c>
-      <c r="G4" s="76" t="s">
-        <v>260</v>
-      </c>
-      <c r="H4" s="74" t="s">
-        <v>231</v>
-      </c>
-      <c r="I4" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="74"/>
-      <c r="K4" s="77"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="66">
-        <v>2</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="66">
-        <v>6</v>
-      </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5">
-      <c r="A6" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
@@ -4693,62 +4586,62 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="72"/>
+      <c r="K6" s="71"/>
     </row>
     <row r="7" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A7" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" s="74" t="s">
+      <c r="A7" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="73"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="65">
+        <v>3</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="65">
+        <v>7</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="77"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="66">
-        <v>3</v>
-      </c>
-      <c r="C8" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="66">
-        <v>7</v>
-      </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="70"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
@@ -4756,58 +4649,58 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="72"/>
+      <c r="K9" s="71"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A10" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="D10" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="77"/>
+      <c r="A10" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="76"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66" t="s">
-        <v>280</v>
-      </c>
-      <c r="D11" s="66">
+      <c r="B11" s="65"/>
+      <c r="C11" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="65">
         <v>8</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69"/>
     </row>
     <row r="12" spans="1:11" ht="25.5">
-      <c r="A12" s="71" t="s">
-        <v>20</v>
+      <c r="A12" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="64" t="s">
-        <v>272</v>
+      <c r="C12" s="63" t="s">
+        <v>262</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9"/>
@@ -4815,56 +4708,56 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="72"/>
+      <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A13" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="78" t="s">
-        <v>247</v>
-      </c>
-      <c r="D13" s="74" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="77"/>
+      <c r="A13" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>219</v>
+      </c>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="76"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="66">
+      <c r="B14" s="65"/>
+      <c r="C14" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="65">
         <v>15</v>
       </c>
-      <c r="E14" s="66"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="70"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="69"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="71" t="s">
-        <v>20</v>
+      <c r="A15" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -4872,51 +4765,51 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="72"/>
+      <c r="K15" s="71"/>
     </row>
     <row r="16" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A16" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="74" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="E16" s="78"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="77"/>
+      <c r="A16" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="77"/>
+      <c r="C16" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" s="77"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="76"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="70"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="69"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="71" t="s">
-        <v>20</v>
+      <c r="A18" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -4925,43 +4818,43 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="72"/>
+      <c r="K18" s="71"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="74" t="s">
-        <v>261</v>
-      </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="77"/>
+      <c r="A19" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="77"/>
+      <c r="C19" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="70"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="71" t="s">
-        <v>20</v>
+      <c r="A21" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -4972,41 +4865,41 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="72"/>
+      <c r="K21" s="71"/>
     </row>
     <row r="22" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A22" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="77"/>
+      <c r="A22" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="77"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="76"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="70"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="71" t="s">
-        <v>20</v>
+      <c r="A24" s="70" t="s">
+        <v>19</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -5017,25 +4910,25 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="72"/>
+      <c r="K24" s="71"/>
     </row>
     <row r="25" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A25" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="77"/>
+      <c r="A25" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="77"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="76"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="56" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="9"/>
@@ -5045,17 +4938,17 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="59"/>
+      <c r="K26" s="58"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="59"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K27" s="60"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -5064,67 +4957,67 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="62"/>
+      <c r="K28" s="61"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="54"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="59"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K30" s="60"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="62"/>
+      <c r="K31" s="61"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="54"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="59"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K33" s="60"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -5134,32 +5027,32 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="62"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="54"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="59"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K36" s="60"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -5169,32 +5062,32 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="62"/>
+      <c r="K37" s="61"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="54"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="57" t="s">
+      <c r="A39" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="59"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K39" s="60"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -5205,32 +5098,32 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="62"/>
+      <c r="K40" s="61"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
-      <c r="K41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="54"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="59"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="60" t="s">
         <v>20</v>
-      </c>
-      <c r="K42" s="60"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="61" t="s">
-        <v>21</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -5241,7 +5134,7 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="62"/>
+      <c r="K43" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5268,7 +5161,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5325,7 +5218,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5333,7 +5226,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5341,7 +5234,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed on color for initial state
</commit_message>
<xml_diff>
--- a/Livestream.xlsx
+++ b/Livestream.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livestream\go\pkg\mod\github.com\lobosat\APCvmix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corsatx.sharepoint.com/sites/Livestream/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B4CFC6-6890-4241-9701-A60452058736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{C8B4CFC6-6890-4241-9701-A60452058736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A016837B-0189-48B9-97D2-F671A8058180}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="2115" windowWidth="18900" windowHeight="12315" tabRatio="844" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="2460" windowWidth="18900" windowHeight="12315" tabRatio="844" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hymns" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="314">
   <si>
     <t>Button</t>
   </si>
@@ -468,88 +468,7 @@
     <t>HebrewStart</t>
   </si>
   <si>
-    <t>Lift every voice and sing till earth and heaven ring
-Ring with the harmonies of Liberty
-Let our rejoicing rise high as the listening skies
-Let it resound loud as the rolling sea</t>
-  </si>
-  <si>
-    <t>Opening Hymn: Lift every voice LEVAS II #1</t>
-  </si>
-  <si>
-    <t>Sing a song full of the faith that the dark past has taught us
-Sing a song full of the hope that the present has brought us
-Facing the rising sun of our new day begun
-Let us march on till victory is won</t>
-  </si>
-  <si>
-    <t>God of our weary years, God of our silent tears
-Thou who has brought us thus far on the way
-Thou who has by Thy might Led us into the light
-Keep us forever in the path, we pray</t>
-  </si>
-  <si>
-    <t>Stony the road we trod, bitter the chastening rod
-Felt in the days when hope unborn had died
-Yet with a steady beat have not our weary feet
-Come to the place for which our fathers sighed?</t>
-  </si>
-  <si>
-    <t>We have come over a way that with tears has been watered
-We have come, treading our path through the blood of the slaughtered
-Out from the gloomy past till now we stand at last
-Where the white gleam of our bright star is cast</t>
-  </si>
-  <si>
-    <t>Lest our feet stray from the places, our God, where we met Thee
-Lest, our hearts drunk with the wine of the world, we forget Thee
-Shadowed beneath Thy hand may we forever stand
-True to our God, true to our native land</t>
-  </si>
-  <si>
-    <t>With the Lord there is mercy, and fullness of redemption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From out of the depths, I cry unto you, Lord, Hear my voice, come hear my prayer;
-O let your ear be open to my pleading. </t>
-  </si>
-  <si>
-    <t>If you, O Lord, should mark our guilt, 
-then who could stand within your sight?
-But in you is found forgiveness for our failings</t>
-  </si>
-  <si>
-    <t>Just as those who wait for the morning light,
-Even more I long for the Lord, my God
-Whose word to me shall ever be my comfort.</t>
-  </si>
-  <si>
-    <t>Offertory Anthem:  One Faith, One Hope, One Lord     Craig Courtney</t>
-  </si>
-  <si>
-    <t>One faith, one hope, one Lord, one church for which He died,
-One voice, one song we lift in praise to him who was, and is, and shall be ever more.</t>
-  </si>
-  <si>
-    <t>There is one body, one spirit, as you were called to one hope. 
-One Lord, baptism and faith, one God and Father of all, who is in you all.</t>
-  </si>
-  <si>
-    <t>Though we be many people, diverse with various gifts, we are given to each other for the unity of faith, that we grow in the knowledge of the Son of God, in the fullness of Christ.</t>
-  </si>
-  <si>
     <t>Lyrics 2</t>
-  </si>
-  <si>
-    <t>Psalm 130  (G127)</t>
-  </si>
-  <si>
-    <t>2 Samuel 1:1, 17-27
-Lector: Mark Mangus</t>
-  </si>
-  <si>
-    <t>2 Corinthians 8:7-15
-Lector: Laureen Cate</t>
   </si>
   <si>
     <t>EpistleStart</t>
@@ -615,19 +534,6 @@
 You are our God. We worship you.</t>
   </si>
   <si>
-    <t>Prayers of the People
-Intercessor: Mark Mangus</t>
-  </si>
-  <si>
-    <t>May they know us by our love.</t>
-  </si>
-  <si>
-    <t>For their love remains with us always.</t>
-  </si>
-  <si>
-    <t>We thank you, O Lover of Souls, for blessings too many to count!  We pray our circle of love ever expands, ever welcomes, and ever seeks to become like the One we receive.  Amen.</t>
-  </si>
-  <si>
     <t>ScriptStart Value=allOff</t>
   </si>
   <si>
@@ -663,47 +569,6 @@
     <t>Forgive us our sins as we forgive those who sin against us. Save us from the time of trial, and deliver us from evil. For the kingdom, the power, and the glory are yours, now and forever. Amen.</t>
   </si>
   <si>
-    <t>Communion Music: O Love that will not let me go</t>
-  </si>
-  <si>
-    <t>Oh love that will not let me go I rest my weary soul in thee
-I give thee back the life I owe that in thine ocean depths its flow may richer, fuller be.</t>
-  </si>
-  <si>
-    <t>Oh light that follows all my way I yield my flickering torch to thee
-My heart restores its borrowed ray that in thy sunshine's blaze its day may brighter, fairer be.</t>
-  </si>
-  <si>
-    <t>Oh joy that seeks me through pain I cannot close my heart to thee
-I trace the rainbow through the rain and feel the promise is not vain that morn shall tearless be</t>
-  </si>
-  <si>
-    <t>Oh cross that’s lifting up my head I dare not ask to fly from thee
-I lay in dust's life's glory dead and from the ground there blossoms red life that shall endless bleed.</t>
-  </si>
-  <si>
-    <t>And we sing Holy, Holy is the king of kings (repeat)</t>
-  </si>
-  <si>
-    <t>Closing Hymn: #411 - O Bless the Lord, My Soul</t>
-  </si>
-  <si>
-    <t>O bless the Lord, my soul! His grace to thee proclaim!
-And all that is within me join to bless his holy name!</t>
-  </si>
-  <si>
-    <t>O bless the Lord, my soul! His mercies bear in mind!
-Forget not all his benefits! The Lord to thee is kind.</t>
-  </si>
-  <si>
-    <t>He clothes us with his love; Upholds us with his truth;
-He heals all our infirmities and ransoms us from death.</t>
-  </si>
-  <si>
-    <t>Then bless his holy name, whose grace hath made us whole,
-Whose loving kindness crowns our days! O bless the Lord, my soul!</t>
-  </si>
-  <si>
     <t>Therefore let us keep the feast. Alleluia.</t>
   </si>
   <si>
@@ -775,9 +640,6 @@
   </si>
   <si>
     <t>leds off 20</t>
-  </si>
-  <si>
-    <t>The Rev. Joshua Woods</t>
   </si>
   <si>
     <t>leds off 23</t>
@@ -925,6 +787,285 @@
   </si>
   <si>
     <t>Offertory Anthem</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynEM</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynAltar</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynChoir1</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynChoir2</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynChoir3</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=setDynSolo</t>
+  </si>
+  <si>
+    <t>ScriptStart Value=micsOff</t>
+  </si>
+  <si>
+    <t>InputDynamic1</t>
+  </si>
+  <si>
+    <t>on: 73</t>
+  </si>
+  <si>
+    <t>off: 73</t>
+  </si>
+  <si>
+    <t>on: 74</t>
+  </si>
+  <si>
+    <t>on: 76</t>
+  </si>
+  <si>
+    <t>off: 76</t>
+  </si>
+  <si>
+    <t>off: 74</t>
+  </si>
+  <si>
+    <t>on: 77</t>
+  </si>
+  <si>
+    <t>off: 77</t>
+  </si>
+  <si>
+    <t>on: 78</t>
+  </si>
+  <si>
+    <t>off: 78</t>
+  </si>
+  <si>
+    <t>on: 79</t>
+  </si>
+  <si>
+    <t>off: 79</t>
+  </si>
+  <si>
+    <t>Dynamic1</t>
+  </si>
+  <si>
+    <t>Prelude</t>
+  </si>
+  <si>
+    <t>Opening Hymn:God Bless America</t>
+  </si>
+  <si>
+    <t>While the storm clouds gather far across the sea,
+Let us swear allegiance to a land that’s free.
+Let us all be grateful for a land so fair
+As we raise our voice in a solemn prayer</t>
+  </si>
+  <si>
+    <t>God bless America, land that I love
+Stand beside her and guide her
+Through the night with the light from above</t>
+  </si>
+  <si>
+    <t>From the mountains to the prairies
+To the oceans white with foam
+God bless America, my home sweet home
+God bless America, my home sweet home!</t>
+  </si>
+  <si>
+    <t>Psalm 123  (G122)</t>
+  </si>
+  <si>
+    <t>Our eyes are fixed on the Lord, pleading for his mercy.</t>
+  </si>
+  <si>
+    <t>To you I have lifted up my eyes, you who dwell in the heavens;
+My eyes, like the eyes of slaves on the hand of their lords.</t>
+  </si>
+  <si>
+    <t>Like the eyes of a servant on the hand of her mistress,
+So our eyes are on the Lord our God till we are shown mercy.</t>
+  </si>
+  <si>
+    <t>Have mercy on us Lord, have mercy.  We are filled with contempt.
+Indeed all too full is our soul with the scorn of the rich, the disdain of the proud.</t>
+  </si>
+  <si>
+    <t>For our families, friends, and neighbors, and for those who are alone.</t>
+  </si>
+  <si>
+    <t>For all who work for justice, freedom, and peace.</t>
+  </si>
+  <si>
+    <t>For the victims of hunger, fear, injustice, and oppression.</t>
+  </si>
+  <si>
+    <t>For those who minister to the sick, the friendless, and the needy.</t>
+  </si>
+  <si>
+    <t>For all who proclaim the Gospel, and all who seek the Truth.</t>
+  </si>
+  <si>
+    <t>For all who serve God in the Church.</t>
+  </si>
+  <si>
+    <t>For your mercy is great.</t>
+  </si>
+  <si>
+    <t>And praise your Name for ever and ever.</t>
+  </si>
+  <si>
+    <t>Who put their trust in you.</t>
+  </si>
+  <si>
+    <t>Offertory Anthem - I am but a Small Voice
+By Odina E. Batnag</t>
+  </si>
+  <si>
+    <t>I am but a small voice, I have but a small dream:  
+The fragrance of a flower in the unpolluted air.
+I am but a small voice, I have but a small dream:  
+To smile upon the sun, be free to dance and sing everywhere.</t>
+  </si>
+  <si>
+    <t>Come, young citizens of the world; we are one.
+We have one hope, we have one dream, and with once voice we sing.
+Give us peace, prosperity, and love for all mankind.</t>
+  </si>
+  <si>
+    <t>] I am but a small voice, I have but a small dream:  
+The fragrance of a flower in the unpolluted air.
+I am but a small voice, I have but a small dream:  
+To smile upon the sun, be free to dance and sing everywhere.</t>
+  </si>
+  <si>
+    <t>Communion Music: Instrumental
+Cindy Sanchez, Flute</t>
+  </si>
+  <si>
+    <t>This is my song, O God of all the nations,
+A song of peace for lands afar and mine. 
+This is my home, the country where my heart is;</t>
+  </si>
+  <si>
+    <t>Closing Hymn - This is My Song (Finlandia)</t>
+  </si>
+  <si>
+    <t>Here are my hopes, my dreams, my holy shrine;
+But other hearts in other lands are beating
+With hopes and dreams as true and high as mine</t>
+  </si>
+  <si>
+    <t>My country's skies are bluer than the ocean, 
+And sunlight beams on cloverleaf and pine.
+But other lands have sunlight too and clover,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And skies are everywhere as blue as mine. 
+Oh, hear my song, O God of all the nations,
+A song of peace for their land and for mine. </t>
+  </si>
+  <si>
+    <t>Patriotic</t>
+  </si>
+  <si>
+    <t>Battle Hymn of the Republic</t>
+  </si>
+  <si>
+    <t>Glory, Glory hallelujah, Glory, Glory hallelujah, Glory, Glory hallelujah
+His truth is marching on</t>
+  </si>
+  <si>
+    <t>America the Beautiful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America! America! God shed His grace on thee, 
+And crown thy good with brotherhood from sea to shining sea! </t>
+  </si>
+  <si>
+    <t>O beautiful for pilgrim feet whose stern impassioned stress, 
+A thoroughfare for freedom beat across the wilderness!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America! America! God mend thine every flaw, 
+Confirm thy soul in self-control, Thy liberty in law! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">America! America! God shed His grace on thee, 
+And crown thy good with brotherhood from sea to shining sea!	</t>
+  </si>
+  <si>
+    <t>SetText Input=Patriotic&amp;SelectedName=TextBlock2.Text&amp;Value=
+OverlayInput4In Input=Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mine eyes have seen the glory of the coming of the Lord
+He is trampling out the vintage where the grapes of wrath are stored
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have seen him in the watch-fires of a hundred circling camps
+They have builded him an altar in the evening dews and damps
+</t>
+  </si>
+  <si>
+    <t>I have read his righteous sentence by the dim and flaring lamps
+His truth is marching on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O beautiful for spacious skies, for amber waves of grain,
+For purple mountain majesties above the fruited plain! </t>
+  </si>
+  <si>
+    <t>O beautiful for patriot dream that sees beyond the years,
+Thine alabaster cities gleam Undimmed by human tears!</t>
+  </si>
+  <si>
+    <t>He has loosed the fateful lightening of his terrible swift sword
+His truth is marching on</t>
+  </si>
+  <si>
+    <t>2 Samuel 5:1-5, 9-10
+Lector: Margaret Lewis</t>
+  </si>
+  <si>
+    <t>2 Corinthians 12:2-10 
+Lector: Sam Gilliam</t>
+  </si>
+  <si>
+    <t>The Rev. Judith Rhodes</t>
+  </si>
+  <si>
+    <t>Prayers of the People
+Intercessor: Art Ramseur</t>
+  </si>
+  <si>
+    <t>leds off 1</t>
+  </si>
+  <si>
+    <t>leds off 2</t>
+  </si>
+  <si>
+    <t>SetText Input=Patriotic&amp;SelectedName=TextBlock2.Text&amp;Value=Prelude - Patriotic Medley %0APlease Sing Along!
+leds yellowBlink 55</t>
+  </si>
+  <si>
+    <t>PoP Next</t>
+  </si>
+  <si>
+    <t>Next
+AudioOn Input=Behringer 3</t>
+  </si>
+  <si>
+    <t>AudioOff Input=Behringer 3</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>mics off</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1317,9 +1458,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1861,222 +1999,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804F0BF0-44B3-4553-A5BB-CBA05E193E99}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="44.140625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="47" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="47" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="47" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="47" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="47" customWidth="1"/>
-    <col min="8" max="8" width="41" style="47" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="43"/>
+    <col min="2" max="2" width="44.140625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="46" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="46" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="41" style="46" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" style="43" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1">
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:9" ht="13.5" thickBot="1">
+      <c r="B1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="45" t="s">
+      <c r="I1" s="43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="40" t="s">
+      <c r="D2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A3" s="46" t="s">
+      <c r="G2" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>9</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="42">
         <v>18</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="42">
         <v>33</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="42">
         <v>37</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>39</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="42">
         <v>41</v>
       </c>
-      <c r="H3" s="48">
+      <c r="H3" s="47">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="51">
-      <c r="B4" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>268</v>
-      </c>
-      <c r="F4" s="51" t="s">
-        <v>269</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75">
-      <c r="B5" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="76.5">
-      <c r="B6" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="51">
-      <c r="B7" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="76.5">
-      <c r="B8" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="76.5">
-      <c r="B9" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="76.5">
-      <c r="B10" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="25.5">
-      <c r="C11" s="47" t="s">
-        <v>148</v>
+      <c r="I3" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51">
+      <c r="B4" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="89.25">
+      <c r="B5" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="63.75">
+      <c r="B6" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="89.25">
+      <c r="B7" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>280</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="63.75">
+      <c r="C8" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="38.25">
+      <c r="C9" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51">
+      <c r="C10" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25.5">
+      <c r="C11" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="51">
+      <c r="I12" s="46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="38.25">
+      <c r="I13" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="51">
+      <c r="I14" s="46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25.5">
+      <c r="I15" s="46" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="51">
+      <c r="I16" s="46" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" ht="38.25">
+      <c r="I17" s="46" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2089,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFA0029-6F67-4CFC-9DD5-769ABDA5C3FC}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2113,11 +2288,17 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
@@ -2355,7 +2536,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2401,7 +2582,7 @@
         <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2654,12 +2835,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" t="s">
+        <v>312</v>
+      </c>
+      <c r="C81" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2674,7 +2861,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2712,8 +2899,8 @@
       <c r="D2" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>158</v>
+      <c r="E2" s="37" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
@@ -2727,10 +2914,10 @@
         <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>159</v>
+        <v>142</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2744,10 +2931,10 @@
         <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>227</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.5">
@@ -2761,10 +2948,10 @@
         <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>177</v>
+        <v>144</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2774,10 +2961,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2792,151 +2979,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="49"/>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="48"/>
+      <c r="B1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="49" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="50" t="s">
+      <c r="D2" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="49" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="49">
         <v>24</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50">
+      <c r="C3" s="49"/>
+      <c r="D3" s="49">
         <v>25</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50">
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="165.75">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="51" t="s">
+      <c r="B4" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="G4" s="51" t="s">
-        <v>240</v>
+      <c r="E4" s="50"/>
+      <c r="G4" s="50" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="63.75">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="50"/>
+      <c r="B5" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="49"/>
       <c r="D5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" s="50"/>
-      <c r="G5" s="50" t="s">
-        <v>241</v>
+        <v>268</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="G5" s="49" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="63.75">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" s="50"/>
+      <c r="B6" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="49"/>
       <c r="D6" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
+        <v>269</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
     </row>
     <row r="7" spans="1:7" ht="76.5">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="50"/>
+      <c r="B7" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="49"/>
       <c r="D7" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-    </row>
-    <row r="8" spans="1:7">
+        <v>270</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5">
       <c r="D8" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
       <c r="D9" s="4" t="s">
-        <v>178</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="D10" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="25.5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="D11" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="76.5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5">
       <c r="D12" s="4" t="s">
-        <v>180</v>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2954,7 +3145,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2967,272 +3158,272 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="H2" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="H3" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="A4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="25"/>
-      <c r="H2" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="F4" s="24"/>
+      <c r="H4" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
+      <c r="A5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="24" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="H5" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="H3" s="26" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="H6" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
+      <c r="A7" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="H7" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
+      <c r="A8" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="H8" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
+      <c r="A9" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="H4" s="26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="A5" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="H5" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15">
-      <c r="A6" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="H6" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="A7" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="H7" s="26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
-      <c r="A8" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="H8" s="26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15">
-      <c r="A9" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="23" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="H9" s="26" t="s">
+      <c r="F9" s="24"/>
+      <c r="H9" s="25" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="23" t="s">
+      <c r="B10" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="H10" s="26" t="s">
+      <c r="F10" s="24"/>
+      <c r="H10" s="25" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="23" t="s">
+      <c r="B11" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="H11" s="26" t="s">
+      <c r="F11" s="24"/>
+      <c r="H11" s="25" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="23" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="H12" s="26" t="s">
+      <c r="F12" s="24"/>
+      <c r="H12" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="23" t="s">
+      <c r="B13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="H13" s="26" t="s">
+      <c r="F13" s="24"/>
+      <c r="H13" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" thickBot="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="25"/>
-      <c r="H14" s="26" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="24"/>
+      <c r="H14" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="25"/>
-      <c r="H15" s="26" t="s">
+      <c r="A15" s="24"/>
+      <c r="H15" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="25"/>
-      <c r="H16" s="26" t="s">
+      <c r="A16" s="24"/>
+      <c r="H16" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3268,44 +3459,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F3" t="s">
@@ -3316,16 +3507,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F4" t="s">
@@ -3336,16 +3527,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F5" t="s">
@@ -3356,16 +3547,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F6" t="s">
@@ -3376,16 +3567,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F7" t="s">
@@ -3396,44 +3587,44 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="33" t="s">
         <v>117</v>
       </c>
       <c r="F10" t="s">
@@ -3442,35 +3633,35 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="1"/>
-      <c r="C11" s="36"/>
+      <c r="C11" s="35"/>
       <c r="F11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" s="1"/>
-      <c r="C12" s="36"/>
+      <c r="C12" s="35"/>
       <c r="F12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="1"/>
-      <c r="C13" s="36"/>
+      <c r="C13" s="35"/>
       <c r="F13" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" s="1"/>
-      <c r="C14" s="36"/>
+      <c r="C14" s="35"/>
       <c r="F14" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" s="1"/>
-      <c r="C15" s="36"/>
+      <c r="C15" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -3516,10 +3707,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3527,10 +3718,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3538,7 +3729,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -3549,7 +3740,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>132</v>
@@ -3560,10 +3751,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3571,10 +3762,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3582,10 +3773,10 @@
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3593,10 +3784,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3604,10 +3795,10 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3615,10 +3806,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
         <v>167</v>
-      </c>
-      <c r="C11" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="38.25">
@@ -3626,10 +3817,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>190</v>
+        <v>149</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3637,10 +3828,10 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3648,10 +3839,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3666,16 +3857,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:IW90"/>
+  <dimension ref="A1:IW82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="14"/>
-    <col min="2" max="2" width="34.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="36" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="14" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" style="10" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="10"/>
@@ -3689,7 +3880,7 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -3699,21 +3890,33 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="63.75">
       <c r="A2" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="B2" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51">
       <c r="A3" s="14">
         <v>2</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>128</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -3725,7 +3928,7 @@
       <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="36" t="s">
         <v>129</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -3737,7 +3940,7 @@
       <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="36" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -3749,20 +3952,20 @@
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>183</v>
+      <c r="B7" s="36" t="s">
+        <v>161</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="25.5">
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>182</v>
+      <c r="B8" s="36" t="s">
+        <v>160</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>65</v>
@@ -3774,8 +3977,8 @@
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>181</v>
+      <c r="B9" s="36" t="s">
+        <v>159</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>63</v>
@@ -3787,8 +3990,8 @@
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>256</v>
+      <c r="B10" s="36" t="s">
+        <v>222</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>78</v>
@@ -3844,8 +4047,8 @@
       <c r="A19" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="37" t="s">
-        <v>254</v>
+      <c r="B19" s="36" t="s">
+        <v>220</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>43</v>
@@ -3863,14 +4066,14 @@
       <c r="A21" s="14">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>164</v>
+      <c r="B21" s="36" t="s">
+        <v>146</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3888,18 +4091,18 @@
         <v>23</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="14">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>255</v>
+      <c r="B25" s="36" t="s">
+        <v>221</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>5</v>
@@ -3910,26 +4113,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="25.5">
       <c r="A27" s="14">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>72</v>
+      <c r="B27" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="14">
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>230</v>
+      <c r="B28" s="36" t="s">
+        <v>196</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3961,11 +4170,11 @@
       <c r="A34" s="14">
         <v>33</v>
       </c>
-      <c r="B34" s="37" t="s">
-        <v>259</v>
+      <c r="B34" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3987,11 +4196,11 @@
       <c r="A38" s="14">
         <v>37</v>
       </c>
-      <c r="B38" s="37" t="s">
-        <v>267</v>
+      <c r="B38" s="36" t="s">
+        <v>233</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>39</v>
@@ -4006,11 +4215,11 @@
       <c r="A40" s="14">
         <v>39</v>
       </c>
-      <c r="B40" s="37" t="s">
-        <v>267</v>
+      <c r="B40" s="36" t="s">
+        <v>233</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>45</v>
@@ -4025,8 +4234,8 @@
       <c r="A42" s="14">
         <v>41</v>
       </c>
-      <c r="B42" s="37" t="s">
-        <v>260</v>
+      <c r="B42" s="36" t="s">
+        <v>226</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>126</v>
@@ -4036,11 +4245,11 @@
       <c r="A43" s="14">
         <v>42</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>255</v>
+      <c r="B43" s="36" t="s">
+        <v>221</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4067,11 +4276,11 @@
       <c r="A48" s="14">
         <v>47</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>239</v>
+      <c r="B48" s="36" t="s">
+        <v>205</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -4083,8 +4292,8 @@
       <c r="A50" s="14">
         <v>49</v>
       </c>
-      <c r="B50" s="37" t="s">
-        <v>261</v>
+      <c r="B50" s="36" t="s">
+        <v>227</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>47</v>
@@ -4099,14 +4308,14 @@
       <c r="A52" s="14">
         <v>51</v>
       </c>
-      <c r="B52" s="15" t="s">
-        <v>243</v>
+      <c r="B52" s="36" t="s">
+        <v>209</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -4125,7 +4334,7 @@
       <c r="A55" s="14">
         <v>54</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="36" t="s">
         <v>71</v>
       </c>
       <c r="D55" s="14"/>
@@ -4134,7 +4343,7 @@
       <c r="A56" s="14">
         <v>55</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="36" t="s">
         <v>72</v>
       </c>
       <c r="D56" s="14"/>
@@ -4143,7 +4352,7 @@
       <c r="A57" s="14">
         <v>56</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="36" t="s">
         <v>73</v>
       </c>
       <c r="D57" s="14"/>
@@ -4158,7 +4367,7 @@
       <c r="A59" s="14">
         <v>58</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="36" t="s">
         <v>57</v>
       </c>
       <c r="D59" s="14"/>
@@ -4167,7 +4376,7 @@
       <c r="A60" s="14">
         <v>59</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="36" t="s">
         <v>58</v>
       </c>
       <c r="D60" s="14"/>
@@ -4176,7 +4385,7 @@
       <c r="A61" s="14">
         <v>60</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="36" t="s">
         <v>59</v>
       </c>
       <c r="D61" s="14"/>
@@ -4197,77 +4406,77 @@
       <c r="A64" s="14">
         <v>63</v>
       </c>
-      <c r="B64" s="15" t="s">
-        <v>244</v>
+      <c r="B64" s="36" t="s">
+        <v>210</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="14">
         <v>64</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>246</v>
+      <c r="B65" s="36" t="s">
+        <v>212</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="14">
         <v>65</v>
       </c>
-      <c r="B66" s="15" t="s">
-        <v>205</v>
+      <c r="B66" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="14">
         <v>66</v>
       </c>
-      <c r="B67" s="15" t="s">
-        <v>206</v>
+      <c r="B67" s="36" t="s">
+        <v>173</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="14">
         <v>67</v>
       </c>
-      <c r="B68" s="15" t="s">
-        <v>207</v>
+      <c r="B68" s="36" t="s">
+        <v>174</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="14">
         <v>68</v>
       </c>
-      <c r="B69" s="15" t="s">
-        <v>208</v>
+      <c r="B69" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="14">
         <v>69</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>209</v>
+      <c r="B70" s="36" t="s">
+        <v>176</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -4275,15 +4484,15 @@
         <v>70</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="14">
         <v>71</v>
       </c>
-      <c r="B72" s="15" t="s">
-        <v>217</v>
+      <c r="B72" s="36" t="s">
+        <v>184</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>114</v>
@@ -4293,22 +4502,28 @@
       <c r="A73" s="14">
         <v>72</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="36" t="s">
         <v>16</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>216</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="14">
         <v>73</v>
       </c>
+      <c r="B74" s="36" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="14">
         <v>74</v>
       </c>
+      <c r="B75" s="36" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="14">
@@ -4319,75 +4534,50 @@
       <c r="A77" s="14">
         <v>76</v>
       </c>
+      <c r="B77" s="36" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="14">
         <v>77</v>
       </c>
+      <c r="B78" s="36" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="14">
         <v>78</v>
       </c>
+      <c r="B79" s="36" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="14">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" s="36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" s="14">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" s="14">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="14">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="14">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="14">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="14">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="14">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="14">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="14">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="14">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4397,10 +4587,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4414,11 +4604,13 @@
     <col min="8" max="8" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="1026" width="8.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="5" customWidth="1"/>
+    <col min="13" max="1026" width="8.7109375" style="5" customWidth="1"/>
     <col min="1027" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" thickBot="1">
+    <row r="1" spans="1:12" ht="13.5" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -4452,130 +4644,145 @@
       <c r="K1" s="5" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="64" t="s">
+      <c r="L1" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="65">
+      <c r="B2" s="64">
         <v>1</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="65">
+      <c r="D2" s="64">
         <v>5</v>
       </c>
-      <c r="E2" s="65">
+      <c r="E2" s="64">
         <v>26</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="70" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="G3" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" s="57" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="I3" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="51" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="9"/>
-      <c r="K3" s="71"/>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A4" s="72" t="s">
+      <c r="K3" s="70"/>
+      <c r="L3" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A4" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="73" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="74" t="s">
-        <v>249</v>
-      </c>
-      <c r="G4" s="75" t="s">
-        <v>250</v>
-      </c>
-      <c r="H4" s="73" t="s">
-        <v>221</v>
-      </c>
-      <c r="I4" s="73" t="s">
+      <c r="E4" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="H4" s="72" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="64" t="s">
+      <c r="J4" s="72"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="64">
         <v>2</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="64">
         <v>6</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="69"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5">
-      <c r="A6" s="70" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="25.5">
+      <c r="A6" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="63" t="s">
-        <v>224</v>
+      <c r="C6" s="62" t="s">
+        <v>191</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>25</v>
@@ -4586,59 +4793,68 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="71"/>
-    </row>
-    <row r="7" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A7" s="72" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A7" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="73" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" s="73" t="s">
+      <c r="C7" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="73"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="64" t="s">
+      <c r="E7" s="72"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="65">
+      <c r="B8" s="64">
         <v>3</v>
       </c>
-      <c r="C8" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="65">
+      <c r="C8" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="64">
         <v>7</v>
       </c>
-      <c r="E8" s="65"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="69"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="70" t="s">
+      <c r="E8" s="64"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="52" t="s">
-        <v>233</v>
+      <c r="C9" s="51" t="s">
+        <v>199</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>27</v>
@@ -4649,58 +4865,67 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="71"/>
-    </row>
-    <row r="10" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A10" s="72" t="s">
+      <c r="K9" s="70"/>
+      <c r="L9" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A10" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="78" t="s">
-        <v>234</v>
-      </c>
-      <c r="D10" s="73" t="s">
+      <c r="C10" s="77" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="76"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="64" t="s">
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="D11" s="65">
+      <c r="B11" s="64"/>
+      <c r="C11" s="64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="64">
         <v>8</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="69"/>
-    </row>
-    <row r="12" spans="1:11" ht="25.5">
-      <c r="A12" s="70" t="s">
+      <c r="E11" s="64"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="25.5">
+      <c r="A12" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="63" t="s">
-        <v>262</v>
+      <c r="C12" s="62" t="s">
+        <v>228</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>218</v>
+        <v>185</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9"/>
@@ -4708,56 +4933,65 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="71"/>
-    </row>
-    <row r="13" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A13" s="72" t="s">
+      <c r="K12" s="70"/>
+      <c r="L12" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A13" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="77" t="s">
-        <v>237</v>
-      </c>
-      <c r="D13" s="73" t="s">
-        <v>219</v>
-      </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="76"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="64" t="s">
+      <c r="B13" s="72"/>
+      <c r="C13" s="76" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="72" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="64">
         <v>15</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="69"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="70" t="s">
+      <c r="E14" s="64"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -4765,51 +4999,60 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="71"/>
-    </row>
-    <row r="16" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A16" s="72" t="s">
+      <c r="K15" s="70"/>
+      <c r="L15" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A16" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="D16" s="73" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" s="77"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="76"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="64" t="s">
+      <c r="B16" s="76"/>
+      <c r="C16" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="76"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="69"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="70" t="s">
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -4818,42 +5061,48 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="71"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A19" s="72" t="s">
+      <c r="K18" s="70"/>
+      <c r="L18" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A19" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="73" t="s">
-        <v>251</v>
-      </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="76"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="64" t="s">
+      <c r="B19" s="76"/>
+      <c r="C19" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="69"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="70" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="9"/>
@@ -4865,40 +5114,40 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="71"/>
-    </row>
-    <row r="22" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A22" s="72" t="s">
+      <c r="K21" s="70"/>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="76"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="64" t="s">
+      <c r="B22" s="76"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="75"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="70" t="s">
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="68"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="69" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="9"/>
@@ -4910,25 +5159,25 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
-      <c r="K24" s="71"/>
-    </row>
-    <row r="25" spans="1:11" ht="13.5" thickBot="1">
-      <c r="A25" s="72" t="s">
+      <c r="K24" s="70"/>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" thickBot="1">
+      <c r="A25" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="76"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="56" t="s">
+      <c r="B25" s="76"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="75"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="55" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="9"/>
@@ -4938,16 +5187,16 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="58"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="56" t="s">
+      <c r="K26" s="57"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="59"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="60" t="s">
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="8"/>
@@ -4957,66 +5206,66 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="61"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="53" t="s">
+      <c r="K28" s="60"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="54"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="56" t="s">
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K30" s="59"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="60" t="s">
+      <c r="K30" s="58"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="61"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="53" t="s">
+      <c r="K31" s="60"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="53"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K33" s="59"/>
+      <c r="K33" s="58"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="8"/>
@@ -5027,31 +5276,31 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="61"/>
+      <c r="K34" s="60"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="53"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K36" s="59"/>
+      <c r="K36" s="58"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B37" s="8"/>
@@ -5062,31 +5311,31 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="61"/>
+      <c r="K37" s="60"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="53"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K39" s="59"/>
+      <c r="K39" s="58"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B40" s="8"/>
@@ -5098,31 +5347,31 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="61"/>
+      <c r="K40" s="60"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="53"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K42" s="59"/>
+      <c r="K42" s="58"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="59" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="8"/>
@@ -5134,7 +5383,7 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="61"/>
+      <c r="K43" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5151,7 +5400,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5211,7 +5460,9 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">

</xml_diff>